<commit_message>
First fully working version
</commit_message>
<xml_diff>
--- a/04 Software/_Examples/Color converter RGB565.xlsx
+++ b/04 Software/_Examples/Color converter RGB565.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hj.vanderpol\Documents\IOT\waarBORGfonds\04 Software\_Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263676B2-427C-4660-9FE7-3B6EF8E3BEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1648DB8-ADD1-40D1-9985-40F137ED0FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>RGB888</t>
   </si>
@@ -90,15 +90,9 @@
     <t>labels</t>
   </si>
   <si>
-    <t>grey</t>
-  </si>
-  <si>
     <t>RGB</t>
   </si>
   <si>
-    <t>A3FF12</t>
-  </si>
-  <si>
     <t>green_radar</t>
   </si>
   <si>
@@ -120,10 +114,13 @@
     <t>small_text</t>
   </si>
   <si>
-    <t>yellow</t>
-  </si>
-  <si>
-    <t>FFFF00</t>
+    <t>FF0000</t>
+  </si>
+  <si>
+    <t>light grey</t>
+  </si>
+  <si>
+    <t>808080</t>
   </si>
 </sst>
 </file>
@@ -256,7 +253,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,12 +338,6 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -393,7 +384,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -440,9 +431,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -513,16 +501,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF808080"/>
+      <color rgb="FF820000"/>
+      <color rgb="FFC0C0C0"/>
+      <color rgb="FFE0E0E0"/>
+      <color rgb="FFFF0000"/>
       <color rgb="FFFFFF00"/>
       <color rgb="FFA00000"/>
-      <color rgb="FF808080"/>
       <color rgb="FF282828"/>
       <color rgb="FF404040"/>
       <color rgb="FF008000"/>
-      <color rgb="FF00C000"/>
-      <color rgb="FFFF0000"/>
-      <color rgb="FF800000"/>
-      <color rgb="FF0594FF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1873,8 +1861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1892,7 +1880,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>0</v>
@@ -1949,38 +1937,38 @@
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2">
-        <f>HEX2DEC(MID($E3,1,2))</f>
+        <f t="shared" ref="F3:F10" si="0">HEX2DEC(MID($E3,1,2))</f>
         <v>0</v>
       </c>
       <c r="G3" s="2">
-        <f>HEX2DEC(MID($E3,3,2))</f>
+        <f t="shared" ref="G3:G10" si="1">HEX2DEC(MID($E3,3,2))</f>
         <v>0</v>
       </c>
       <c r="H3" s="2">
-        <f>HEX2DEC(MID($E3,5,2))</f>
+        <f t="shared" ref="H3:H10" si="2">HEX2DEC(MID($E3,5,2))</f>
         <v>0</v>
       </c>
       <c r="I3" s="2">
-        <f>_xlfn.BITRSHIFT(F3,3)</f>
+        <f t="shared" ref="I3:I10" si="3">_xlfn.BITRSHIFT(F3,3)</f>
         <v>0</v>
       </c>
       <c r="J3" s="2">
-        <f>_xlfn.BITRSHIFT(G3,2)</f>
+        <f t="shared" ref="J3:J10" si="4">_xlfn.BITRSHIFT(G3,2)</f>
         <v>0</v>
       </c>
       <c r="K3" s="2">
-        <f>_xlfn.BITRSHIFT(H3,3)</f>
+        <f t="shared" ref="K3:K10" si="5">_xlfn.BITRSHIFT(H3,3)</f>
         <v>0</v>
       </c>
       <c r="L3" s="2" t="str">
-        <f>DEC2HEX(_xlfn.BITLSHIFT(I3,11)+_xlfn.BITLSHIFT(J3,5)+K3,4)</f>
+        <f t="shared" ref="L3:L10" si="6">DEC2HEX(_xlfn.BITLSHIFT(I3,11)+_xlfn.BITLSHIFT(J3,5)+K3,4)</f>
         <v>0000</v>
       </c>
       <c r="M3" s="8" t="str">
-        <f>"#define CLR_"&amp;LEFT(UPPER(B3)&amp;REPT(" ",$M$1),$M$1)&amp;" 0x"&amp;L3&amp;"   // "&amp;DEC2HEX(F3,2)&amp;", "&amp;DEC2HEX(G3,2)&amp;", "&amp;DEC2HEX(H3,2)&amp;" = "&amp;C3</f>
+        <f t="shared" ref="M3:M10" si="7">"#define CLR_"&amp;LEFT(UPPER(B3)&amp;REPT(" ",$M$1),$M$1)&amp;" 0x"&amp;L3&amp;"   // "&amp;DEC2HEX(F3,2)&amp;", "&amp;DEC2HEX(G3,2)&amp;", "&amp;DEC2HEX(H3,2)&amp;" = "&amp;C3</f>
         <v>#define CLR_BACKGROUND   0x0000   // 00, 00, 00 = black</v>
       </c>
     </row>
@@ -1999,35 +1987,35 @@
         <v>282828</v>
       </c>
       <c r="F4" s="2">
-        <f>HEX2DEC(MID($E4,1,2))</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="G4" s="2">
-        <f>HEX2DEC(MID($E4,3,2))</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="H4" s="2">
-        <f>HEX2DEC(MID($E4,5,2))</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="I4" s="2">
-        <f>_xlfn.BITRSHIFT(F4,3)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="J4" s="2">
-        <f>_xlfn.BITRSHIFT(G4,2)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="K4" s="2">
-        <f>_xlfn.BITRSHIFT(H4,3)</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="L4" s="2" t="str">
-        <f>DEC2HEX(_xlfn.BITLSHIFT(I4,11)+_xlfn.BITLSHIFT(J4,5)+K4,4)</f>
+        <f t="shared" si="6"/>
         <v>2945</v>
       </c>
       <c r="M4" s="8" t="str">
-        <f>"#define CLR_"&amp;LEFT(UPPER(B4)&amp;REPT(" ",$M$1),$M$1)&amp;" 0x"&amp;L4&amp;"   // "&amp;DEC2HEX(F4,2)&amp;", "&amp;DEC2HEX(G4,2)&amp;", "&amp;DEC2HEX(H4,2)&amp;" = "&amp;C4</f>
+        <f t="shared" si="7"/>
         <v>#define CLR_DARK         0x2945   // 28, 28, 28 = dark grey</v>
       </c>
     </row>
@@ -2046,35 +2034,35 @@
         <v>8</v>
       </c>
       <c r="F5" s="2">
-        <f>HEX2DEC(MID($E5,1,2))</f>
+        <f t="shared" si="0"/>
         <v>255</v>
       </c>
       <c r="G5" s="2">
-        <f>HEX2DEC(MID($E5,3,2))</f>
+        <f t="shared" si="1"/>
         <v>255</v>
       </c>
       <c r="H5" s="2">
-        <f>HEX2DEC(MID($E5,5,2))</f>
+        <f t="shared" si="2"/>
         <v>255</v>
       </c>
       <c r="I5" s="2">
-        <f>_xlfn.BITRSHIFT(F5,3)</f>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="J5" s="2">
-        <f>_xlfn.BITRSHIFT(G5,2)</f>
+        <f t="shared" si="4"/>
         <v>63</v>
       </c>
       <c r="K5" s="2">
-        <f>_xlfn.BITRSHIFT(H5,3)</f>
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
       <c r="L5" s="2" t="str">
-        <f>DEC2HEX(_xlfn.BITLSHIFT(I5,11)+_xlfn.BITLSHIFT(J5,5)+K5,4)</f>
+        <f t="shared" si="6"/>
         <v>FFFF</v>
       </c>
       <c r="M5" s="8" t="str">
-        <f>"#define CLR_"&amp;LEFT(UPPER(B5)&amp;REPT(" ",$M$1),$M$1)&amp;" 0x"&amp;L5&amp;"   // "&amp;DEC2HEX(F5,2)&amp;", "&amp;DEC2HEX(G5,2)&amp;", "&amp;DEC2HEX(H5,2)&amp;" = "&amp;C5</f>
+        <f t="shared" si="7"/>
         <v>#define CLR_TEXT         0xFFFF   // FF, FF, FF = white</v>
       </c>
     </row>
@@ -2083,46 +2071,46 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="16" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F6" s="2">
-        <f>HEX2DEC(MID($E6,1,2))</f>
-        <v>163</v>
+        <f t="shared" si="0"/>
+        <v>255</v>
       </c>
       <c r="G6" s="2">
-        <f>HEX2DEC(MID($E6,3,2))</f>
-        <v>255</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="H6" s="2">
-        <f>HEX2DEC(MID($E6,5,2))</f>
-        <v>18</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="I6" s="2">
-        <f>_xlfn.BITRSHIFT(F6,3)</f>
-        <v>20</v>
+        <f t="shared" si="3"/>
+        <v>31</v>
       </c>
       <c r="J6" s="2">
-        <f>_xlfn.BITRSHIFT(G6,2)</f>
-        <v>63</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="K6" s="2">
-        <f>_xlfn.BITRSHIFT(H6,3)</f>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="L6" s="2" t="str">
-        <f>DEC2HEX(_xlfn.BITLSHIFT(I6,11)+_xlfn.BITLSHIFT(J6,5)+K6,4)</f>
-        <v>A7E2</v>
+        <f t="shared" si="6"/>
+        <v>F800</v>
       </c>
       <c r="M6" s="14" t="str">
-        <f>"#define CLR_"&amp;LEFT(UPPER(B6)&amp;REPT(" ",$M$1),$M$1)&amp;" 0x"&amp;L6&amp;"   // "&amp;DEC2HEX(F6,2)&amp;", "&amp;DEC2HEX(G6,2)&amp;", "&amp;DEC2HEX(H6,2)&amp;" = "&amp;C6</f>
-        <v>#define CLR_RADAR_WIPER  0xA7E2   // A3, FF, 12 = red</v>
+        <f t="shared" si="7"/>
+        <v>#define CLR_RADAR_WIPER  0xF800   // FF, 00, 00 = red</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -2133,43 +2121,43 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="16">
-        <v>808080</v>
+        <v>15</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="F7" s="2">
-        <f>HEX2DEC(MID($E7,1,2))</f>
-        <v>128</v>
+        <f t="shared" si="0"/>
+        <v>255</v>
       </c>
       <c r="G7" s="2">
-        <f>HEX2DEC(MID($E7,3,2))</f>
-        <v>128</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="H7" s="2">
-        <f>HEX2DEC(MID($E7,5,2))</f>
-        <v>128</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="I7" s="2">
-        <f>_xlfn.BITRSHIFT(F7,3)</f>
-        <v>16</v>
+        <f t="shared" si="3"/>
+        <v>31</v>
       </c>
       <c r="J7" s="2">
-        <f>_xlfn.BITRSHIFT(G7,2)</f>
-        <v>32</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="K7" s="2">
-        <f>_xlfn.BITRSHIFT(H7,3)</f>
-        <v>16</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="L7" s="2" t="str">
-        <f>DEC2HEX(_xlfn.BITLSHIFT(I7,11)+_xlfn.BITLSHIFT(J7,5)+K7,4)</f>
-        <v>8410</v>
+        <f t="shared" si="6"/>
+        <v>F800</v>
       </c>
       <c r="M7" s="8" t="str">
-        <f>"#define CLR_"&amp;LEFT(UPPER(B7)&amp;REPT(" ",$M$1),$M$1)&amp;" 0x"&amp;L7&amp;"   // "&amp;DEC2HEX(F7,2)&amp;", "&amp;DEC2HEX(G7,2)&amp;", "&amp;DEC2HEX(H7,2)&amp;" = "&amp;C7</f>
-        <v>#define CLR_LABELS       0x8410   // 80, 80, 80 = grey</v>
+        <f t="shared" si="7"/>
+        <v>#define CLR_LABELS       0xF800   // FF, 00, 00 = red</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -2177,45 +2165,45 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
         <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F8" s="2">
-        <f>HEX2DEC(MID($E8,1,2))</f>
+        <f t="shared" si="0"/>
         <v>160</v>
       </c>
       <c r="G8" s="2">
-        <f>HEX2DEC(MID($E8,3,2))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H8" s="2">
-        <f>HEX2DEC(MID($E8,5,2))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I8" s="2">
-        <f>_xlfn.BITRSHIFT(F8,3)</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="J8" s="2">
-        <f>_xlfn.BITRSHIFT(G8,2)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K8" s="2">
-        <f>_xlfn.BITRSHIFT(H8,3)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L8" s="2" t="str">
-        <f>DEC2HEX(_xlfn.BITLSHIFT(I8,11)+_xlfn.BITLSHIFT(J8,5)+K8,4)</f>
+        <f t="shared" si="6"/>
         <v>A000</v>
       </c>
       <c r="M8" s="8" t="str">
-        <f>"#define CLR_"&amp;LEFT(UPPER(B8)&amp;REPT(" ",$M$1),$M$1)&amp;" 0x"&amp;L8&amp;"   // "&amp;DEC2HEX(F8,2)&amp;", "&amp;DEC2HEX(G8,2)&amp;", "&amp;DEC2HEX(H8,2)&amp;" = "&amp;C8</f>
+        <f t="shared" si="7"/>
         <v>#define CLR_RED_RADAR    0xA000   // A0, 00, 00 = dark red</v>
       </c>
     </row>
@@ -2224,7 +2212,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>16</v>
@@ -2234,80 +2222,80 @@
         <v>17</v>
       </c>
       <c r="F9" s="2">
-        <f>HEX2DEC(MID($E9,1,2))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G9" s="2">
-        <f>HEX2DEC(MID($E9,3,2))</f>
+        <f t="shared" si="1"/>
         <v>128</v>
       </c>
       <c r="H9" s="2">
-        <f>HEX2DEC(MID($E9,5,2))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I9" s="2">
-        <f>_xlfn.BITRSHIFT(F9,3)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J9" s="2">
-        <f>_xlfn.BITRSHIFT(G9,2)</f>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="K9" s="2">
-        <f>_xlfn.BITRSHIFT(H9,3)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L9" s="2" t="str">
-        <f>DEC2HEX(_xlfn.BITLSHIFT(I9,11)+_xlfn.BITLSHIFT(J9,5)+K9,4)</f>
+        <f t="shared" si="6"/>
         <v>0400</v>
       </c>
       <c r="M9" s="8" t="str">
-        <f>"#define CLR_"&amp;LEFT(UPPER(B9)&amp;REPT(" ",$M$1),$M$1)&amp;" 0x"&amp;L9&amp;"   // "&amp;DEC2HEX(F9,2)&amp;", "&amp;DEC2HEX(G9,2)&amp;", "&amp;DEC2HEX(H9,2)&amp;" = "&amp;C9</f>
+        <f t="shared" si="7"/>
         <v>#define CLR_GREEN_RADAR  0x0400   // 00, 80, 00 = green</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="13"/>
+      <c r="E10" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="16" t="s">
-        <v>30</v>
-      </c>
       <c r="F10" s="2">
-        <f>HEX2DEC(MID($E10,1,2))</f>
-        <v>255</v>
+        <f t="shared" si="0"/>
+        <v>128</v>
       </c>
       <c r="G10" s="2">
-        <f>HEX2DEC(MID($E10,3,2))</f>
-        <v>255</v>
+        <f t="shared" si="1"/>
+        <v>128</v>
       </c>
       <c r="H10" s="2">
-        <f>HEX2DEC(MID($E10,5,2))</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>128</v>
       </c>
       <c r="I10" s="2">
-        <f>_xlfn.BITRSHIFT(F10,3)</f>
-        <v>31</v>
+        <f t="shared" si="3"/>
+        <v>16</v>
       </c>
       <c r="J10" s="2">
-        <f>_xlfn.BITRSHIFT(G10,2)</f>
-        <v>63</v>
+        <f t="shared" si="4"/>
+        <v>32</v>
       </c>
       <c r="K10" s="2">
-        <f>_xlfn.BITRSHIFT(H10,3)</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
       <c r="L10" s="2" t="str">
-        <f>DEC2HEX(_xlfn.BITLSHIFT(I10,11)+_xlfn.BITLSHIFT(J10,5)+K10,4)</f>
-        <v>FFE0</v>
+        <f t="shared" si="6"/>
+        <v>8410</v>
       </c>
       <c r="M10" s="8" t="str">
-        <f>"#define CLR_"&amp;LEFT(UPPER(B10)&amp;REPT(" ",$M$1),$M$1)&amp;" 0x"&amp;L10&amp;"   // "&amp;DEC2HEX(F10,2)&amp;", "&amp;DEC2HEX(G10,2)&amp;", "&amp;DEC2HEX(H10,2)&amp;" = "&amp;C10</f>
-        <v>#define CLR_SMALL_TEXT   0xFFE0   // FF, FF, 00 = yellow</v>
+        <f t="shared" si="7"/>
+        <v>#define CLR_SMALL_TEXT   0x8410   // 80, 80, 80 = light grey</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>